<commit_message>
feat: too many refactors for one commit
</commit_message>
<xml_diff>
--- a/docs/db-design-2023-09-28.xlsx
+++ b/docs/db-design-2023-09-28.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t xml:space="preserve">users</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">INTEGER NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">story_main</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +215,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,7 +306,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -418,8 +429,12 @@
       <c r="F13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
+      <c r="A14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="F14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>